<commit_message>
nieuwe lineare regressie voor SmoothRank
</commit_message>
<xml_diff>
--- a/measurements/ranklib_test.xlsx
+++ b/measurements/ranklib_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
   <si>
     <t>NDCG@10</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>MapRed</t>
+  </si>
+  <si>
+    <t>MSLR-WEB30k (20 epochs)</t>
   </si>
 </sst>
 </file>
@@ -105,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -121,6 +127,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,21 +410,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="10" customWidth="1"/>
+    <col min="8" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -431,14 +440,17 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
         <v>1</v>
@@ -458,15 +470,21 @@
       <c r="J2" t="s">
         <v>0</v>
       </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
       <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
       <c r="B3" s="3"/>
       <c r="C3">
         <v>1</v>
@@ -486,15 +504,21 @@
       <c r="J3">
         <v>0.1744</v>
       </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
       <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
+        <v>0.1837</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>0.46329999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
       <c r="B4" s="3"/>
       <c r="C4">
         <v>2</v>
@@ -514,15 +538,21 @@
       <c r="J4">
         <v>0.18210000000000001</v>
       </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
       <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
+        <v>0.18310000000000001</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
         <v>0.42209999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
       <c r="B5" s="3"/>
       <c r="C5">
         <v>3</v>
@@ -542,15 +572,21 @@
       <c r="J5">
         <v>0.1837</v>
       </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
       <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5">
+        <v>0.1835</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
         <v>0.43169999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="C6">
         <v>4</v>
@@ -570,15 +606,21 @@
       <c r="J6">
         <v>0.17660000000000001</v>
       </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
       <c r="M6">
-        <v>4</v>
-      </c>
-      <c r="N6">
+        <v>0.18149999999999999</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
         <v>0.40670000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7">
         <v>5</v>
@@ -598,15 +640,21 @@
       <c r="J7">
         <v>0.18429999999999999</v>
       </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
       <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7">
+        <v>0.184</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
         <v>0.44290000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
         <v>3</v>
@@ -629,16 +677,22 @@
         <f>AVERAGE(J3:J7)</f>
         <v>0.18021999999999999</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8">
-        <f>AVERAGE(N3:N7)</f>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>1498.933</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <f>AVERAGE(Q3:Q7)</f>
         <v>0.43334</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5" t="s">
         <v>9</v>
@@ -657,15 +711,238 @@
         <v>24167</v>
       </c>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N9" s="6"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="4"/>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="4"/>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="4"/>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="P16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="4"/>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="e">
+        <f>AVERAGE(G13:G17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" t="e">
+        <f>AVERAGE(J13:J17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" t="e">
+        <f>AVERAGE(Q13:Q17)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19">
+        <v>41736.214999999997</v>
+      </c>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:A9"/>
+    <mergeCell ref="A11:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>